<commit_message>
Actualizando HU y MVH
</commit_message>
<xml_diff>
--- a/DESARROLLO/SAV/GESTION/SAV-HU.xlsx
+++ b/DESARROLLO/SAV/GESTION/SAV-HU.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF5C380-4593-4A20-A1D4-1CA6D2406F06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55154C5-8DF4-4BE9-BAE3-105A920B20E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="HU-Estudiante" sheetId="1" r:id="rId1"/>
+    <sheet name="HU-Docente" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="243">
   <si>
     <t>ENUNCIADO DE LA HISTORIA</t>
   </si>
@@ -726,13 +727,31 @@
   </si>
   <si>
     <t>Visualizar tareas Asignadas</t>
+  </si>
+  <si>
+    <t>Necesito poder eleminar estudiante</t>
+  </si>
+  <si>
+    <t>Con la finalidad de poder eliminar de la lista alumnos que ya no van a evaluarse</t>
+  </si>
+  <si>
+    <t>El sistema muestra la opcion de eliminar estudiante</t>
+  </si>
+  <si>
+    <t>En caso el docente haya ingresado en la opcion de visualizar estudiantes</t>
+  </si>
+  <si>
+    <t>Cuando haya presionado en el icono de eliminar estudiante</t>
+  </si>
+  <si>
+    <t>H30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -780,6 +799,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -816,7 +842,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -848,17 +874,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -872,6 +889,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1213,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1234,15 +1293,15 @@
     <row r="1" spans="1:9" ht="26.4" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="15"/>
+      <c r="G1" s="28"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
@@ -1272,19 +1331,19 @@
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="79.8" customHeight="1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="26" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="5">
@@ -1297,11 +1356,11 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="5">
         <v>2</v>
       </c>
@@ -1312,11 +1371,11 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
       <c r="F5" s="5">
         <v>3</v>
       </c>
@@ -1327,11 +1386,11 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
       <c r="F6" s="5">
         <v>4</v>
       </c>
@@ -1342,19 +1401,19 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="79.8" customHeight="1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="26" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="5">
@@ -1367,11 +1426,11 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="5">
         <v>2</v>
       </c>
@@ -1382,11 +1441,11 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
       <c r="F9" s="5">
         <v>3</v>
       </c>
@@ -1397,19 +1456,19 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="33.6" customHeight="1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="26" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="5">
@@ -1422,11 +1481,11 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="5">
         <v>2</v>
       </c>
@@ -1437,11 +1496,11 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="30.6" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="5">
         <v>3</v>
       </c>
@@ -1452,11 +1511,11 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="34.799999999999997" customHeight="1">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="5">
         <v>4</v>
       </c>
@@ -1467,19 +1526,19 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="119.4" customHeight="1">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="26" t="s">
         <v>35</v>
       </c>
       <c r="F14" s="5">
@@ -1492,11 +1551,11 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="26.4">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="5">
         <v>2</v>
       </c>
@@ -1507,11 +1566,11 @@
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" ht="26.4">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="5">
         <v>3</v>
       </c>
@@ -1522,19 +1581,19 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" ht="93" customHeight="1">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="26" t="s">
         <v>42</v>
       </c>
       <c r="F17" s="5">
@@ -1547,11 +1606,11 @@
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
       <c r="F18" s="5">
         <v>2</v>
       </c>
@@ -1562,11 +1621,11 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="5">
         <v>3</v>
       </c>
@@ -1577,11 +1636,11 @@
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
       <c r="F20" s="5">
         <v>4</v>
       </c>
@@ -1592,11 +1651,11 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
       <c r="F21" s="5">
         <v>5</v>
       </c>
@@ -1632,19 +1691,19 @@
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" ht="106.2" customHeight="1">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="26" t="s">
         <v>56</v>
       </c>
       <c r="F23" s="5">
@@ -1657,11 +1716,11 @@
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
       <c r="F24" s="5">
         <v>2</v>
       </c>
@@ -1672,11 +1731,11 @@
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
       <c r="F25" s="5">
         <v>3</v>
       </c>
@@ -1687,11 +1746,11 @@
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="13"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
       <c r="F26" s="5">
         <v>4</v>
       </c>
@@ -1727,19 +1786,19 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" ht="26.4">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="26" t="s">
         <v>69</v>
       </c>
       <c r="F28" s="5">
@@ -1752,11 +1811,11 @@
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="5">
         <v>2</v>
       </c>
@@ -1767,11 +1826,11 @@
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" ht="26.4">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
       <c r="F30" s="5">
         <v>3</v>
       </c>
@@ -1782,11 +1841,11 @@
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" ht="26.4">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
       <c r="F31" s="5">
         <v>4</v>
       </c>
@@ -1797,11 +1856,11 @@
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" ht="26.4">
-      <c r="A32" s="13"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
       <c r="F32" s="5">
         <v>5</v>
       </c>
@@ -1812,11 +1871,11 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
       <c r="F33" s="5">
         <v>6</v>
       </c>
@@ -1827,11 +1886,11 @@
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" ht="33" customHeight="1">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
       <c r="F34" s="5">
         <v>7</v>
       </c>
@@ -1842,19 +1901,19 @@
       <c r="I34" s="2"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="26" t="s">
         <v>80</v>
       </c>
       <c r="F35" s="5">
@@ -1867,11 +1926,11 @@
       <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" ht="26.4">
-      <c r="A36" s="13"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
       <c r="F36" s="5">
         <v>2</v>
       </c>
@@ -1882,11 +1941,11 @@
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
       <c r="F37" s="5">
         <v>3</v>
       </c>
@@ -1897,19 +1956,19 @@
       <c r="I37" s="2"/>
     </row>
     <row r="38" spans="1:9" ht="119.4" customHeight="1">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="26" t="s">
         <v>87</v>
       </c>
       <c r="F38" s="5">
@@ -1922,11 +1981,11 @@
       <c r="I38" s="2"/>
     </row>
     <row r="39" spans="1:9" ht="26.4">
-      <c r="A39" s="13"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
       <c r="F39" s="5">
         <v>2</v>
       </c>
@@ -1937,11 +1996,11 @@
       <c r="I39" s="2"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="13"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
       <c r="F40" s="5">
         <v>3</v>
       </c>
@@ -1952,11 +2011,11 @@
       <c r="I40" s="2"/>
     </row>
     <row r="41" spans="1:9" ht="26.4">
-      <c r="A41" s="13"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
       <c r="F41" s="5">
         <v>4</v>
       </c>
@@ -1992,19 +2051,19 @@
       <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" ht="106.2" customHeight="1">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="E43" s="13" t="s">
+      <c r="E43" s="26" t="s">
         <v>56</v>
       </c>
       <c r="F43" s="5">
@@ -2017,11 +2076,11 @@
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="13"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
       <c r="F44" s="5">
         <v>2</v>
       </c>
@@ -2032,11 +2091,11 @@
       <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="13"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
       <c r="F45" s="5">
         <v>3</v>
       </c>
@@ -2047,11 +2106,11 @@
       <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="13"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
       <c r="F46" s="5">
         <v>4</v>
       </c>
@@ -2062,19 +2121,19 @@
       <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:9" ht="106.2" customHeight="1">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="26" t="s">
         <v>103</v>
       </c>
       <c r="F47" s="5">
@@ -2087,11 +2146,11 @@
       <c r="I47" s="2"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="13"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
       <c r="F48" s="5">
         <v>2</v>
       </c>
@@ -2102,11 +2161,11 @@
       <c r="I48" s="2"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="13"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
       <c r="F49" s="5">
         <v>3</v>
       </c>
@@ -2117,11 +2176,11 @@
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="13"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
       <c r="F50" s="5">
         <v>4</v>
       </c>
@@ -2132,11 +2191,11 @@
       <c r="I50" s="2"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="13"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
       <c r="F51" s="5">
         <v>5</v>
       </c>
@@ -2147,11 +2206,11 @@
       <c r="I51" s="2"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="13"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
       <c r="F52" s="5">
         <v>6</v>
       </c>
@@ -2162,11 +2221,11 @@
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="13"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
       <c r="F53" s="5">
         <v>7</v>
       </c>
@@ -2177,11 +2236,11 @@
       <c r="I53" s="2"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="13"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
       <c r="F54" s="5">
         <v>8</v>
       </c>
@@ -2192,19 +2251,19 @@
       <c r="I54" s="2"/>
     </row>
     <row r="55" spans="1:9" ht="91.8" customHeight="1">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E55" s="26" t="s">
         <v>115</v>
       </c>
       <c r="F55" s="5">
@@ -2217,11 +2276,11 @@
       <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="13"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
       <c r="F56" s="5">
         <v>2</v>
       </c>
@@ -2268,672 +2327,312 @@
       <c r="I58" s="2"/>
     </row>
     <row r="59" spans="1:9" ht="27.6" customHeight="1">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G59" s="15"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
+      <c r="A59" s="20"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
     </row>
     <row r="60" spans="1:9" ht="24.6" customHeight="1">
-      <c r="A60" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="A60" s="21"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
     </row>
     <row r="61" spans="1:9" s="12" customFormat="1" ht="26.4" customHeight="1">
-      <c r="A61" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D61" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="E61" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="F61" s="16">
-        <v>1</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="H61" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="I61" s="16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="27.6">
-      <c r="A62" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="B62" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C62" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D62" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="E62" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="F62" s="16">
-        <v>1</v>
-      </c>
-      <c r="G62" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="H62" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="I62" s="16" t="s">
-        <v>181</v>
-      </c>
+      <c r="A61" s="22"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="22"/>
+      <c r="I61" s="22"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="22"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="22"/>
+      <c r="I62" s="22"/>
     </row>
     <row r="63" spans="1:9" ht="53.4" customHeight="1">
-      <c r="A63" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D63" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="E63" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="F63" s="16">
-        <v>1</v>
-      </c>
-      <c r="G63" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="H63" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="I63" s="16" t="s">
-        <v>187</v>
-      </c>
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="22"/>
     </row>
     <row r="64" spans="1:9" ht="40.200000000000003" customHeight="1">
-      <c r="A64" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B64" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="C64" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D64" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="F64" s="16">
-        <v>1</v>
-      </c>
-      <c r="G64" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="H64" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="I64" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="41.4">
-      <c r="A65" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C65" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D65" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E65" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="F65" s="16">
-        <v>1</v>
-      </c>
-      <c r="G65" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="H65" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="I65" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="41.4">
-      <c r="A66" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="B66" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D66" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="E66" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="F66" s="16">
-        <v>1</v>
-      </c>
-      <c r="G66" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="H66" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="I66" s="16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="41.4">
-      <c r="A67" s="19"/>
-      <c r="B67" s="19"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="16">
-        <v>2</v>
-      </c>
-      <c r="G67" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="H67" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="I67" s="16" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="41.4">
-      <c r="A68" s="19"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="16">
-        <v>3</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="I68" s="16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="27.6">
-      <c r="A69" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="C69" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D69" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="E69" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="F69" s="16">
-        <v>1</v>
-      </c>
-      <c r="G69" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H69" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="I69" s="16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="27.6">
-      <c r="A70" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="B70" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D70" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="F70" s="16">
-        <v>1</v>
-      </c>
-      <c r="G70" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="H70" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="I70" s="16" t="s">
-        <v>184</v>
-      </c>
+      <c r="A64" s="22"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="22"/>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="22"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="22"/>
+      <c r="I65" s="22"/>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="30"/>
+      <c r="B66" s="30"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22"/>
+      <c r="H66" s="22"/>
+      <c r="I66" s="22"/>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="30"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
+      <c r="I67" s="22"/>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="30"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="22"/>
+      <c r="H68" s="22"/>
+      <c r="I68" s="22"/>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="22"/>
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="22"/>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="30"/>
+      <c r="B70" s="30"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+      <c r="H70" s="22"/>
+      <c r="I70" s="22"/>
     </row>
     <row r="71" spans="1:9" ht="62.4" customHeight="1">
-      <c r="A71" s="19"/>
-      <c r="B71" s="19"/>
-      <c r="C71" s="19"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="16">
-        <v>2</v>
-      </c>
-      <c r="G71" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="H71" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="I71" s="16" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="27.6">
-      <c r="A72" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B72" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="C72" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D72" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="E72" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="F72" s="16">
-        <v>1</v>
-      </c>
-      <c r="G72" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="H72" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="I72" s="16" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="41.4">
-      <c r="A73" s="19"/>
-      <c r="B73" s="19"/>
-      <c r="C73" s="19"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="16">
-        <v>2</v>
-      </c>
-      <c r="G73" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="H73" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="I73" s="16" t="s">
-        <v>167</v>
-      </c>
+      <c r="A71" s="30"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="22"/>
+      <c r="I71" s="22"/>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="30"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="30"/>
+      <c r="E72" s="30"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="22"/>
+      <c r="I72" s="22"/>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="30"/>
+      <c r="B73" s="30"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="22"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="22"/>
     </row>
     <row r="74" spans="1:9" ht="63" customHeight="1">
-      <c r="A74" s="19"/>
-      <c r="B74" s="19"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="16">
-        <v>3</v>
-      </c>
-      <c r="G74" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="H74" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="I74" s="16" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="27.6">
-      <c r="A75" s="19"/>
-      <c r="B75" s="19"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="20">
-        <v>4</v>
-      </c>
-      <c r="G75" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="H75" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="I75" s="16" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="27.6">
-      <c r="A76" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B76" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="C76" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="E76" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="F76" s="16">
-        <v>1</v>
-      </c>
-      <c r="G76" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="H76" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="I76" s="16" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="41.4">
-      <c r="A77" s="19"/>
-      <c r="B77" s="19"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="19"/>
-      <c r="E77" s="19"/>
-      <c r="F77" s="16">
-        <v>2</v>
-      </c>
-      <c r="G77" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="H77" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="I77" s="16" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="41.4">
-      <c r="A78" s="19"/>
-      <c r="B78" s="19"/>
-      <c r="C78" s="19"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="16">
-        <v>3</v>
-      </c>
-      <c r="G78" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="H78" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="I78" s="16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="41.4">
-      <c r="A79" s="19"/>
-      <c r="B79" s="19"/>
-      <c r="C79" s="19"/>
-      <c r="D79" s="19"/>
-      <c r="E79" s="19"/>
-      <c r="F79" s="20">
-        <v>4</v>
-      </c>
-      <c r="G79" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="H79" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="I79" s="16" t="s">
-        <v>209</v>
-      </c>
+      <c r="A74" s="30"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="30"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="22"/>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="30"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22"/>
+      <c r="I75" s="22"/>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="30"/>
+      <c r="B76" s="30"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30"/>
+      <c r="F76" s="22"/>
+      <c r="G76" s="22"/>
+      <c r="H76" s="22"/>
+      <c r="I76" s="22"/>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="30"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="30"/>
+      <c r="F77" s="22"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="22"/>
+      <c r="I77" s="22"/>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="30"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="30"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="30"/>
+      <c r="F78" s="22"/>
+      <c r="G78" s="22"/>
+      <c r="H78" s="22"/>
+      <c r="I78" s="22"/>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="30"/>
+      <c r="B79" s="30"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="22"/>
+      <c r="I79" s="22"/>
     </row>
     <row r="80" spans="1:9" ht="33.6" customHeight="1">
-      <c r="A80" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="C80" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="E80" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="F80" s="16">
-        <v>1</v>
-      </c>
-      <c r="G80" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="H80" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="I80" s="16" t="s">
-        <v>227</v>
-      </c>
+      <c r="A80" s="30"/>
+      <c r="B80" s="30"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="22"/>
+      <c r="H80" s="22"/>
+      <c r="I80" s="22"/>
     </row>
     <row r="81" spans="1:9" ht="66" customHeight="1">
-      <c r="A81" s="19"/>
-      <c r="B81" s="19"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="19"/>
-      <c r="E81" s="19"/>
-      <c r="F81" s="16">
-        <v>2</v>
-      </c>
-      <c r="G81" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="H81" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="I81" s="16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="27.6">
-      <c r="A82" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="C82" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D82" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="F82" s="16">
-        <v>1</v>
-      </c>
-      <c r="G82" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="H82" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="I82" s="16" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="41.4">
-      <c r="A83" s="19"/>
-      <c r="B83" s="19"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="19"/>
-      <c r="E83" s="19"/>
-      <c r="F83" s="16">
-        <v>2</v>
-      </c>
-      <c r="G83" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="H83" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="I83" s="16" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="41.4">
-      <c r="A84" s="19"/>
-      <c r="B84" s="19"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="19"/>
-      <c r="E84" s="19"/>
-      <c r="F84" s="16">
-        <v>3</v>
-      </c>
-      <c r="G84" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="H84" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="I84" s="16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="41.4">
-      <c r="A85" s="19"/>
-      <c r="B85" s="19"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="19"/>
-      <c r="F85" s="20">
-        <v>4</v>
-      </c>
-      <c r="G85" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="H85" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="I85" s="16" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="28.8">
-      <c r="A86" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="B86" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="C86" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D86" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="E86" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="F86" s="20">
-        <v>1</v>
-      </c>
-      <c r="G86" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="H86" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="I86" s="16" t="s">
-        <v>235</v>
-      </c>
+      <c r="A81" s="30"/>
+      <c r="B81" s="30"/>
+      <c r="C81" s="30"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
+      <c r="H81" s="22"/>
+      <c r="I81" s="22"/>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="30"/>
+      <c r="B82" s="30"/>
+      <c r="C82" s="30"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="30"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="22"/>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="30"/>
+      <c r="B83" s="30"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="30"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
+      <c r="H83" s="22"/>
+      <c r="I83" s="22"/>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="30"/>
+      <c r="B84" s="30"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="30"/>
+      <c r="F84" s="22"/>
+      <c r="G84" s="22"/>
+      <c r="H84" s="22"/>
+      <c r="I84" s="22"/>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="30"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="22"/>
+      <c r="H85" s="22"/>
+      <c r="I85" s="22"/>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="25"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="22"/>
+      <c r="I86" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="94">
@@ -3036,4 +2735,762 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3B99BE-A015-4D79-BE46-CDA35EAC9465}">
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" customWidth="1"/>
+    <col min="5" max="5" width="61.5546875" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="69.5546875" customWidth="1"/>
+    <col min="8" max="8" width="56.6640625" customWidth="1"/>
+    <col min="9" max="9" width="73.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="28"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="42.6" customHeight="1">
+      <c r="A3" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="16">
+        <v>1</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="54.6" customHeight="1">
+      <c r="A4" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="16">
+        <v>1</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="33" customHeight="1">
+      <c r="A5" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="16">
+        <v>1</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="35.4" customHeight="1">
+      <c r="A6" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" s="16">
+        <v>1</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="37.799999999999997" customHeight="1">
+      <c r="A7" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" s="16">
+        <v>1</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="44.4" customHeight="1">
+      <c r="A8" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45.6" customHeight="1">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="51.6" customHeight="1">
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="16">
+        <v>3</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="42" customHeight="1">
+      <c r="A11" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="16">
+        <v>1</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="32.4" customHeight="1">
+      <c r="A12" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="34.200000000000003" customHeight="1">
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="16">
+        <v>2</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="34.200000000000003" customHeight="1">
+      <c r="A14" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="F14" s="19">
+        <v>1</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="60" customHeight="1">
+      <c r="A15" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="39" customHeight="1">
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="16">
+        <v>2</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="39" customHeight="1">
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="16">
+        <v>3</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45.6" customHeight="1">
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="17">
+        <v>4</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="53.4" customHeight="1">
+      <c r="A19" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="F19" s="16">
+        <v>1</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="35.4" customHeight="1">
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="16">
+        <v>2</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="43.2" customHeight="1">
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="16">
+        <v>3</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="27.6">
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="17">
+        <v>4</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="37.799999999999997" customHeight="1">
+      <c r="A23" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="40.200000000000003" customHeight="1">
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="16">
+        <v>2</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="36.6" customHeight="1">
+      <c r="A25" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="F25" s="16">
+        <v>1</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="32.4" customHeight="1">
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="16">
+        <v>2</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="35.4" customHeight="1">
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="16">
+        <v>3</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="45.6" customHeight="1">
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="17">
+        <v>4</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="35.4" customHeight="1">
+      <c r="A29" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="F29" s="17">
+        <v>1</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="E25:E28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>